<commit_message>
in development: adding labels
</commit_message>
<xml_diff>
--- a/Data/prop plot demo data.xlsx
+++ b/Data/prop plot demo data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/sally_thompson_mlcsu_nhs_uk/Documents/Documents/R scripts/Proportion Plot development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/sally_thompson_mlcsu_nhs_uk/Documents/Documents/R/proportion-plot/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D05E0881-32BC-416A-8E08-7C8DD5E9FB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B44B7A2-2EF3-4C28-97FF-3D3B3F13B7DD}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{D05E0881-32BC-416A-8E08-7C8DD5E9FB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C3137AE-C3E5-42A4-A85B-85277E23B916}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="1815" windowWidth="21330" windowHeight="12510" xr2:uid="{4BD8364A-C636-4E69-95C0-A3C36BAC945E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BD8364A-C636-4E69-95C0-A3C36BAC945E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +434,10 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
-        <v>42</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,10 +445,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -456,10 +456,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -467,10 +467,10 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -478,10 +478,10 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>